<commit_message>
enlarge the tilesize by adding loops along input col dim
</commit_message>
<xml_diff>
--- a/semia_cast_transpose.xlsx
+++ b/semia_cast_transpose.xlsx
@@ -7,7 +7,8 @@
     <workbookView windowWidth="27945" windowHeight="12375"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="results" sheetId="1" r:id="rId1"/>
+    <sheet name="add loops" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="35">
   <si>
     <t>H20</t>
   </si>
@@ -77,6 +78,12 @@
     <t>[16384,8192]</t>
   </si>
   <si>
+    <t>8,4,8,4,loop=2</t>
+  </si>
+  <si>
+    <t>8,4,8,4,loop=4</t>
+  </si>
+  <si>
     <t>[8192,1024]</t>
   </si>
   <si>
@@ -103,6 +110,32 @@
   <si>
     <t>8,8,8,4</t>
   </si>
+  <si>
+    <t>number of subtile : Threads_per_warp</t>
+  </si>
+  <si>
+    <t>subtile:4x2</t>
+  </si>
+  <si>
+    <t>......</t>
+  </si>
+  <si>
+    <t>number of subtile :
+warps_per_tile</t>
+  </si>
+  <si>
+    <t>Loop0</t>
+  </si>
+  <si>
+    <t>Loop1</t>
+  </si>
+  <si>
+    <t>.....</t>
+  </si>
+  <si>
+    <t>number of subtile :
+loop_cnt*warps_per_tile</t>
+  </si>
 </sst>
 </file>
 
@@ -115,12 +148,25 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK SC"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK SC"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -144,12 +190,6 @@
       <sz val="12"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Noto Sans CJK SC"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -309,12 +349,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -324,6 +376,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.0499893185216834"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -492,12 +550,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -533,12 +585,40 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -642,139 +722,133 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -783,68 +857,91 @@
     <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -908,6 +1005,458 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>191135</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>226060</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>108585</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="右大括号 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="7231380" y="2133600"/>
+          <a:ext cx="905510" cy="2718435"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="zh-CN">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>92075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>81915</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>167005</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="右大括号 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="3042285" y="2225675"/>
+          <a:ext cx="901065" cy="6882130"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="zh-CN">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>681990</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104140</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>211455</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>177165</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="右大括号 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="7221220" y="6244590"/>
+          <a:ext cx="901065" cy="2873375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="zh-CN">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1188,10 +1737,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B5:M51"/>
+  <dimension ref="B5:Q51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1200,801 +1749,949 @@
     <col min="4" max="4" width="15.6916666666667" customWidth="1"/>
     <col min="5" max="5" width="11.375" customWidth="1"/>
     <col min="6" max="6" width="14.625" customWidth="1"/>
-    <col min="7" max="7" width="14.4416666666667" customWidth="1"/>
-    <col min="8" max="8" width="18.5" customWidth="1"/>
-    <col min="9" max="9" width="15.4416666666667" customWidth="1"/>
-    <col min="10" max="10" width="12.875" customWidth="1"/>
+    <col min="7" max="11" width="14.4416666666667" customWidth="1"/>
+    <col min="12" max="12" width="18.5" customWidth="1"/>
+    <col min="13" max="13" width="15.4416666666667" customWidth="1"/>
+    <col min="14" max="14" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" ht="15" spans="4:8">
-      <c r="D5" s="3"/>
-      <c r="E5" s="4" t="s">
+    <row r="5" ht="15" spans="4:12">
+      <c r="D5" s="12"/>
+      <c r="E5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="4" t="s">
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" ht="15" spans="2:8">
-      <c r="B6" s="6" t="s">
+    <row r="6" ht="15" spans="2:12">
+      <c r="B6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" ht="15" spans="2:8">
-      <c r="B7" s="3" t="s">
+    <row r="7" ht="15" spans="2:12">
+      <c r="B7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="19">
         <v>57.081</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="20">
         <v>59.81</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7">
         <f>E7/F7</f>
         <v>0.954372178565457</v>
       </c>
     </row>
-    <row r="8" ht="15" spans="2:8">
-      <c r="B8" s="3" t="s">
+    <row r="8" ht="15" spans="2:12">
+      <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="19">
         <v>41.376</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="20">
         <v>44.24</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8">
         <f>E8/F8</f>
         <v>0.935262206148282</v>
       </c>
     </row>
-    <row r="9" ht="15" spans="2:8">
-      <c r="B9" s="3" t="s">
+    <row r="9" ht="15" spans="2:12">
+      <c r="B9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="19">
         <v>22.772</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="20">
         <v>25.74</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9">
         <f>E9/F9</f>
         <v>0.884693084693085</v>
       </c>
     </row>
-    <row r="10" s="1" customFormat="1" ht="15" spans="2:8">
-      <c r="B10" s="12" t="s">
+    <row r="10" s="10" customFormat="1" ht="15" spans="2:12">
+      <c r="B10" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="23">
         <v>272.38</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="23">
         <v>493.71</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="24">
+        <v>545.33</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="24">
+        <v>621.71</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="29">
         <f>E10/F10</f>
         <v>0.551700390917745</v>
       </c>
     </row>
-    <row r="11" ht="15" spans="2:8">
-      <c r="B11" s="3" t="s">
+    <row r="11" ht="15" spans="2:12">
+      <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="10">
+      <c r="D11" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="19">
         <v>23.91</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="20">
         <v>23.29</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11">
         <f>E11/F11</f>
         <v>1.02662086732503</v>
       </c>
     </row>
     <row r="12" ht="15" spans="5:6">
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" ht="15" spans="2:8">
-      <c r="B13" s="3" t="s">
+      <c r="E12" s="19"/>
+      <c r="F12" s="20"/>
+    </row>
+    <row r="13" ht="15" spans="2:12">
+      <c r="B13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="9" t="s">
+      <c r="C13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="19">
         <v>57.154</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="20">
         <v>59.65</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13">
         <f>E13/F13</f>
         <v>0.95815590947192</v>
       </c>
     </row>
-    <row r="14" ht="15" spans="2:8">
-      <c r="B14" s="3" t="s">
+    <row r="14" ht="15" spans="2:12">
+      <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="9" t="s">
+      <c r="C14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="19">
         <v>41.228</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="20">
         <v>51.12</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14">
         <f>E14/F14</f>
         <v>0.806494522691706</v>
       </c>
     </row>
-    <row r="15" ht="15" spans="2:8">
-      <c r="B15" s="3" t="s">
+    <row r="15" ht="15" spans="2:12">
+      <c r="B15" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="9" t="s">
+      <c r="C15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="19">
         <v>22.742</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="20">
         <v>25.83</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15">
         <f>E15/F15</f>
         <v>0.880449090205188</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" ht="15" spans="2:8">
-      <c r="B16" s="12" t="s">
+    <row r="16" s="10" customFormat="1" ht="15" spans="2:12">
+      <c r="B16" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="13" t="s">
+      <c r="C16" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="23">
         <v>272.15</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="23">
         <v>493.36</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="29">
         <f>E16/F16</f>
         <v>0.551625587806065</v>
       </c>
     </row>
-    <row r="17" ht="15" spans="2:8">
-      <c r="B17" s="3" t="s">
+    <row r="17" ht="15" spans="2:12">
+      <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="10">
+      <c r="C17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="19">
         <v>23.99</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="20">
         <v>23.36</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17">
         <f>E17/F17</f>
         <v>1.02696917808219</v>
       </c>
     </row>
-    <row r="19" ht="15" spans="2:7">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="9"/>
+    <row r="19" ht="15" spans="2:11">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="18"/>
       <c r="E19"/>
       <c r="F19"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" ht="15" spans="2:7">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="9"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+    </row>
+    <row r="20" ht="15" spans="2:11">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="18"/>
       <c r="E20"/>
       <c r="F20"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" ht="15" spans="2:10">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5" t="s">
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+    </row>
+    <row r="21" ht="15" spans="2:14">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" ht="15" spans="2:10">
-      <c r="B22" s="17" t="s">
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" ht="15" spans="2:14">
+      <c r="B22" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="18" t="s">
+      <c r="D22" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="M22" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="N22" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" ht="15" spans="2:10">
-      <c r="B23" s="3" t="s">
+    <row r="23" ht="15" spans="2:14">
+      <c r="B23" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="3">
+      <c r="C23" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="12">
         <v>16384</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="12">
         <v>8192</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="28">
         <v>322</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11">
         <v>272.68</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J23" s="21">
-        <f>F23/H23</f>
+      <c r="M23" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="N23" s="30">
+        <f>F23/L23</f>
         <v>1.18087135103418</v>
       </c>
     </row>
-    <row r="24" ht="15" spans="2:10">
-      <c r="B24" s="3" t="s">
+    <row r="24" ht="15" spans="2:14">
+      <c r="B24" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="3">
+      <c r="C24" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="12">
         <v>8192</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="12">
         <v>1024</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="11">
         <v>23.51</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11">
         <v>19.07</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J24" s="21">
-        <f>F24/H24</f>
+      <c r="M24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="N24" s="30">
+        <f>F24/L24</f>
         <v>1.23282642894599</v>
       </c>
     </row>
-    <row r="25" ht="15" spans="2:10">
-      <c r="B25" s="3" t="s">
+    <row r="25" ht="15" spans="2:14">
+      <c r="B25" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="3">
+      <c r="C25" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="12">
         <v>2048</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="12">
         <v>12288</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="11">
         <v>57.95</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11">
         <v>36.91</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J25" s="21">
-        <f>F25/H25</f>
+      <c r="M25" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="N25" s="30">
+        <f>F25/L25</f>
         <v>1.57003522080737</v>
       </c>
     </row>
-    <row r="26" ht="15" spans="2:10">
-      <c r="B26" s="3" t="s">
+    <row r="26" ht="15" spans="2:14">
+      <c r="B26" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="3">
+      <c r="C26" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="12">
         <v>256</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="12">
         <v>65536</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="11">
         <v>44.91</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11">
         <v>27.81</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J26" s="21">
-        <f>F26/H26</f>
+      <c r="M26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="N26" s="30">
+        <f>F26/L26</f>
         <v>1.61488673139159</v>
       </c>
     </row>
-    <row r="27" ht="15" spans="2:10">
-      <c r="B27" s="3" t="s">
+    <row r="27" ht="15" spans="2:14">
+      <c r="B27" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="3">
+      <c r="C27" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="12">
         <v>65536</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="12">
         <v>128</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="11">
         <v>24.23</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11">
         <v>12.24</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J27" s="21">
-        <f>F27/H27</f>
+      <c r="M27" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="N27" s="30">
+        <f>F27/L27</f>
         <v>1.97957516339869</v>
       </c>
     </row>
-    <row r="29" ht="15" spans="2:7">
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="9"/>
+    <row r="29" ht="15" spans="2:11">
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="18"/>
       <c r="E29"/>
       <c r="F29"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" ht="15" spans="2:7">
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="9"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+    </row>
+    <row r="30" ht="15" spans="2:11">
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="18"/>
       <c r="E30"/>
       <c r="F30"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" ht="15" spans="2:7">
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="9"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+    </row>
+    <row r="31" ht="15" spans="2:11">
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="18"/>
       <c r="E31"/>
       <c r="F31"/>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" ht="15" spans="2:7">
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="9"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+    </row>
+    <row r="32" ht="15" spans="2:11">
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="18"/>
       <c r="E32"/>
       <c r="F32"/>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" ht="15" spans="2:7">
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="9"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+    </row>
+    <row r="33" ht="15" spans="2:11">
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="18"/>
       <c r="E33"/>
       <c r="F33"/>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="35" ht="15" spans="2:7">
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="9"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+    </row>
+    <row r="35" ht="15" spans="2:11">
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="18"/>
       <c r="E35"/>
       <c r="F35"/>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" ht="15" spans="2:7">
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="9"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+    </row>
+    <row r="36" ht="15" spans="2:11">
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="18"/>
       <c r="E36"/>
       <c r="F36"/>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" ht="15" spans="2:7">
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="9"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+    </row>
+    <row r="37" ht="15" spans="2:11">
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="18"/>
       <c r="E37"/>
       <c r="F37"/>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" ht="15" spans="2:7">
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="9"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+    </row>
+    <row r="38" ht="15" spans="2:11">
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="18"/>
       <c r="E38"/>
       <c r="F38"/>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" ht="15" spans="2:7">
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="9"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+    </row>
+    <row r="39" ht="15" spans="2:11">
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="18"/>
       <c r="E39"/>
       <c r="F39"/>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="43" s="2" customFormat="1" ht="15" spans="6:9">
-      <c r="F43" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I43" s="5"/>
-    </row>
-    <row r="44" s="2" customFormat="1" ht="15" spans="2:9">
-      <c r="B44" s="17" t="s">
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+    </row>
+    <row r="43" s="11" customFormat="1" ht="15" spans="6:13">
+      <c r="F43" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M43" s="14"/>
+    </row>
+    <row r="44" s="11" customFormat="1" ht="15" spans="2:13">
+      <c r="B44" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C44" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F44" s="18" t="s">
+      <c r="D44" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F44" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="19" t="s">
+      <c r="G44" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="I44" s="19" t="s">
+      <c r="M44" s="27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" s="2" customFormat="1" ht="15" spans="2:9">
-      <c r="B45" s="3" t="s">
+    <row r="45" s="11" customFormat="1" ht="15" spans="2:13">
+      <c r="B45" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D45" s="3">
+      <c r="C45" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="12">
         <v>16384</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="12">
         <v>8192</v>
       </c>
-      <c r="F45" s="20">
+      <c r="F45" s="28">
         <v>322</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G45" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H45" s="2">
+      <c r="L45" s="11">
         <v>272.68</v>
       </c>
-      <c r="I45" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" s="2" customFormat="1" ht="15" spans="2:9">
-      <c r="B46" s="3" t="s">
+      <c r="M45" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" s="11" customFormat="1" ht="15" spans="2:13">
+      <c r="B46" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D46" s="3">
+      <c r="C46" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" s="12">
         <v>8192</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="12">
         <v>1024</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F46" s="11">
         <v>23.51</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G46" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H46" s="2">
+      <c r="L46" s="11">
         <v>19.07</v>
       </c>
-      <c r="I46" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" s="2" customFormat="1" ht="15" spans="2:9">
-      <c r="B47" s="3" t="s">
+      <c r="M46" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" s="11" customFormat="1" ht="15" spans="2:13">
+      <c r="B47" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="3">
+      <c r="C47" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="12">
         <v>2048</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="12">
         <v>12288</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F47" s="11">
         <v>57.95</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G47" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H47" s="2">
+      <c r="L47" s="11">
         <v>36.91</v>
       </c>
-      <c r="I47" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" s="2" customFormat="1" ht="15" spans="2:9">
-      <c r="B48" s="3" t="s">
+      <c r="M47" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" s="11" customFormat="1" ht="15" spans="2:13">
+      <c r="B48" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D48" s="3">
+      <c r="C48" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" s="12">
         <v>256</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="12">
         <v>65536</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F48" s="11">
         <v>44.91</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G48" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H48" s="2">
+      <c r="L48" s="11">
         <v>27.81</v>
       </c>
-      <c r="I48" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" s="2" customFormat="1" ht="15" spans="2:9">
-      <c r="B49" s="3" t="s">
+      <c r="M48" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" s="11" customFormat="1" ht="15" spans="2:13">
+      <c r="B49" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D49" s="3">
+      <c r="C49" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="12">
         <v>65536</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="12">
         <v>128</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F49" s="11">
         <v>24.23</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G49" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H49" s="2">
+      <c r="L49" s="11">
         <v>12.24</v>
       </c>
-      <c r="I49" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" s="2" customFormat="1" ht="15" spans="2:13">
-      <c r="B50" s="3" t="s">
+      <c r="M49" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" s="11" customFormat="1" ht="15" spans="2:17">
+      <c r="B50" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D50" s="3">
+      <c r="C50" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" s="12">
         <v>768</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="12">
         <v>1024</v>
       </c>
-      <c r="F50" s="2">
+      <c r="F50" s="11">
         <v>4.93</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="G50" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H50" s="2">
+      <c r="L50" s="11">
         <v>5.76</v>
       </c>
-      <c r="I50" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M50" s="22"/>
-    </row>
-    <row r="51" s="2" customFormat="1" ht="15" spans="2:9">
-      <c r="B51" s="3" t="s">
+      <c r="M50" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q50" s="31"/>
+    </row>
+    <row r="51" s="11" customFormat="1" ht="15" spans="2:13">
+      <c r="B51" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D51" s="2">
+      <c r="C51" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D51" s="11">
         <v>256</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E51" s="11">
         <v>256</v>
       </c>
-      <c r="F51" s="2">
+      <c r="F51" s="11">
         <v>4.44</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="G51" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H51" s="2">
+      <c r="L51" s="11">
         <v>5.73</v>
       </c>
-      <c r="I51" s="2" t="s">
-        <v>24</v>
+      <c r="M51" s="11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2009,4 +2706,1142 @@
 </oddHeader>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="C4:AI43"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S28" sqref="S28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="2" width="9" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="32.675" customWidth="1"/>
+    <col min="6" max="6" width="35.1416666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" ht="15" spans="3:25">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+    </row>
+    <row r="5" ht="15" spans="3:25">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+    </row>
+    <row r="6" ht="15" spans="3:25">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+    </row>
+    <row r="7" ht="15" spans="3:25">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+    </row>
+    <row r="8" ht="15" spans="3:25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+    </row>
+    <row r="9" ht="20.25" spans="3:25">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+    </row>
+    <row r="10" ht="15" spans="3:25">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+    </row>
+    <row r="11" ht="15" spans="3:25">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+    </row>
+    <row r="12" ht="15" spans="3:35">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="7"/>
+      <c r="AE12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG12" s="5"/>
+      <c r="AH12" s="5"/>
+      <c r="AI12" s="6"/>
+    </row>
+    <row r="13" ht="15" spans="3:35">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="5"/>
+      <c r="AG13" s="5"/>
+      <c r="AH13" s="5"/>
+      <c r="AI13" s="6"/>
+    </row>
+    <row r="14" ht="15" spans="3:35">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="6"/>
+      <c r="AE14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG14" s="7"/>
+      <c r="AH14" s="7"/>
+      <c r="AI14" s="7"/>
+    </row>
+    <row r="15" ht="15" spans="3:35">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="6"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="7"/>
+      <c r="AH15" s="7"/>
+      <c r="AI15" s="7"/>
+    </row>
+    <row r="16" ht="40.5" spans="3:35">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="9"/>
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="9"/>
+      <c r="AI16" s="9"/>
+    </row>
+    <row r="17" ht="15" spans="3:25">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+    </row>
+    <row r="18" ht="15" spans="3:25">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+    </row>
+    <row r="19" ht="15" spans="3:25">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+    </row>
+    <row r="20" ht="15" spans="3:25">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+    </row>
+    <row r="21" ht="15" spans="3:25">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+    </row>
+    <row r="22" ht="15" spans="3:25">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+    </row>
+    <row r="23" ht="15" spans="3:25">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+    </row>
+    <row r="24" ht="15" spans="3:25">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+    </row>
+    <row r="25" ht="15" spans="3:25">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+    </row>
+    <row r="26" ht="50" customHeight="1" spans="3:25">
+      <c r="C26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+    </row>
+    <row r="27" ht="15" spans="3:25">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+    </row>
+    <row r="28" ht="15" spans="3:25">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+    </row>
+    <row r="29" ht="15" spans="3:25">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+    </row>
+    <row r="30" ht="15" spans="3:25">
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+    </row>
+    <row r="31" ht="15" spans="3:25">
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+    </row>
+    <row r="32" ht="15" spans="3:25">
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+    </row>
+    <row r="33" ht="15" spans="3:25">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+    </row>
+    <row r="34" ht="15" spans="3:25">
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+    </row>
+    <row r="35" ht="40.5" spans="3:25">
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+      <c r="Y35" s="1"/>
+    </row>
+    <row r="36" ht="15" spans="3:25">
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+    </row>
+    <row r="37" ht="15" spans="3:25">
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+    </row>
+    <row r="38" ht="15" spans="3:25">
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+    </row>
+    <row r="39" ht="15" spans="3:25">
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
+    </row>
+    <row r="40" ht="15" spans="3:25">
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+      <c r="Y40" s="1"/>
+    </row>
+    <row r="41" ht="15" spans="3:25">
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
+      <c r="X41" s="1"/>
+      <c r="Y41" s="1"/>
+    </row>
+    <row r="42" ht="15" spans="3:25">
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
+      <c r="X42" s="1"/>
+      <c r="Y42" s="1"/>
+    </row>
+    <row r="43" ht="15" spans="3:25">
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+      <c r="Y43" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="J16:V16"/>
+    <mergeCell ref="W16:AI16"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>